<commit_message>
Fixed major bug in lines 101 through 103 where the dataframe was not updating the correct position
</commit_message>
<xml_diff>
--- a/Data-Scraping-Manufacturer-BS/Scrape-Manufacturers/Optifuse/optifuse-original.xlsx
+++ b/Data-Scraping-Manufacturer-BS/Scrape-Manufacturers/Optifuse/optifuse-original.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\48WS-Work\48ws-github\Data-Scraping-Manufacturer-BS\Scrape-Manufacturers\Optifuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C66C7C3-F2C7-4AF5-8AB4-9F7C58CCE8D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF83CE2-848D-4662-B703-63F73937F699}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,8 +389,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,60 +608,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="7.625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="7.625" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="26" width="7.625" customWidth="1"/>
+    <col min="1" max="3" width="7.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="7.625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="26" width="7.625" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -672,13 +673,13 @@
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
@@ -687,13 +688,13 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
@@ -702,13 +703,13 @@
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
@@ -717,10 +718,10 @@
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -731,13 +732,13 @@
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
@@ -746,13 +747,13 @@
       <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
@@ -761,13 +762,13 @@
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="H8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
@@ -776,13 +777,13 @@
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
@@ -791,13 +792,13 @@
       <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
@@ -806,13 +807,13 @@
       <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="H11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
@@ -821,13 +822,13 @@
       <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
@@ -836,13 +837,13 @@
       <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="H13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
@@ -851,13 +852,13 @@
       <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="H14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
@@ -866,13 +867,13 @@
       <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="2" t="s">
+      <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
@@ -881,13 +882,13 @@
       <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="2" t="s">
+      <c r="H16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="2"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
@@ -896,13 +897,13 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="H17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="2"/>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
@@ -911,13 +912,13 @@
       <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="H18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="2"/>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
@@ -926,13 +927,13 @@
       <c r="D19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="H19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
@@ -941,13 +942,13 @@
       <c r="D20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="H20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="2"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
@@ -956,13 +957,13 @@
       <c r="D21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="H21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J21" s="2"/>
+      <c r="J21" s="1"/>
     </row>
     <row r="22" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
@@ -971,13 +972,13 @@
       <c r="D22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="H22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="2"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
@@ -986,13 +987,13 @@
       <c r="D23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="H23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="2"/>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
@@ -1001,13 +1002,13 @@
       <c r="D24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="H24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J24" s="2"/>
+      <c r="J24" s="1"/>
     </row>
     <row r="25" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
@@ -1016,13 +1017,13 @@
       <c r="D25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="H25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J25" s="2"/>
+      <c r="J25" s="1"/>
     </row>
     <row r="26" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
@@ -1031,13 +1032,13 @@
       <c r="D26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="2"/>
+      <c r="J26" s="1"/>
     </row>
     <row r="27" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
@@ -1046,13 +1047,13 @@
       <c r="D27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="H27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J27" s="2"/>
+      <c r="J27" s="1"/>
     </row>
     <row r="28" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
@@ -1061,13 +1062,13 @@
       <c r="D28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="H28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="2"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
@@ -1076,13 +1077,13 @@
       <c r="D29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H29" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="2" t="s">
+      <c r="H29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J29" s="2"/>
+      <c r="J29" s="1"/>
     </row>
     <row r="30" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
@@ -1091,13 +1092,13 @@
       <c r="D30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="H30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J30" s="2"/>
+      <c r="J30" s="1"/>
     </row>
     <row r="31" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
@@ -1106,13 +1107,13 @@
       <c r="D31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="H31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J31" s="2"/>
+      <c r="J31" s="1"/>
     </row>
     <row r="32" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
@@ -1121,13 +1122,13 @@
       <c r="D32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="H32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J32" s="2"/>
+      <c r="J32" s="1"/>
     </row>
     <row r="33" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
@@ -1136,13 +1137,13 @@
       <c r="D33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="H33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J33" s="2"/>
+      <c r="J33" s="1"/>
     </row>
     <row r="34" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
@@ -1151,13 +1152,13 @@
       <c r="D34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="H34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J34" s="2"/>
+      <c r="J34" s="1"/>
     </row>
     <row r="35" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
@@ -1166,13 +1167,13 @@
       <c r="D35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="2" t="s">
+      <c r="H35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J35" s="2"/>
+      <c r="J35" s="1"/>
     </row>
     <row r="36" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
@@ -1181,13 +1182,13 @@
       <c r="D36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H36" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="2" t="s">
+      <c r="H36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J36" s="2"/>
+      <c r="J36" s="1"/>
     </row>
     <row r="37" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
@@ -1196,13 +1197,13 @@
       <c r="D37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="2" t="s">
+      <c r="H37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J37" s="2"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
@@ -1211,13 +1212,13 @@
       <c r="D38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="2" t="s">
+      <c r="H38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J38" s="2"/>
+      <c r="J38" s="1"/>
     </row>
     <row r="39" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
@@ -1226,13 +1227,13 @@
       <c r="D39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="H39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J39" s="2"/>
+      <c r="J39" s="1"/>
     </row>
     <row r="40" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
@@ -1241,13 +1242,13 @@
       <c r="D40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H40" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" s="2" t="s">
+      <c r="H40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J40" s="2"/>
+      <c r="J40" s="1"/>
     </row>
     <row r="41" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
@@ -1256,10 +1257,10 @@
       <c r="D41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H41" t="s">
-        <v>15</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="H41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1270,10 +1271,10 @@
       <c r="D42" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="H42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1284,10 +1285,10 @@
       <c r="D43" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H43" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" t="s">
+      <c r="H43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1298,10 +1299,10 @@
       <c r="D44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H44" t="s">
-        <v>15</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="H44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1312,10 +1313,10 @@
       <c r="D45" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" t="s">
+      <c r="H45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1326,10 +1327,10 @@
       <c r="D46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H46" t="s">
-        <v>15</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="H46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1340,10 +1341,10 @@
       <c r="D47" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H47" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="H47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1556,586 +1557,586 @@
       <c r="D99" s="1"/>
     </row>
     <row r="100" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
     </row>
     <row r="101" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
     </row>
     <row r="102" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
     </row>
     <row r="103" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
     </row>
     <row r="104" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
     </row>
     <row r="105" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
     </row>
     <row r="106" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
     </row>
     <row r="107" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
     </row>
     <row r="108" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
     </row>
     <row r="109" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
     </row>
     <row r="110" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
     </row>
     <row r="111" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
     </row>
     <row r="112" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
     </row>
     <row r="113" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
     </row>
     <row r="114" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
     </row>
     <row r="115" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
     </row>
     <row r="116" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
     </row>
     <row r="117" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
     </row>
     <row r="118" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
     </row>
     <row r="119" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
     </row>
     <row r="120" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
     </row>
     <row r="121" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
     </row>
     <row r="122" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
     </row>
     <row r="123" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
     </row>
     <row r="124" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
     </row>
     <row r="125" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
     </row>
     <row r="126" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
     </row>
     <row r="127" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
     </row>
     <row r="128" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
     </row>
     <row r="129" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
     </row>
     <row r="130" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
     </row>
     <row r="131" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
     </row>
     <row r="132" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
     </row>
     <row r="133" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
+      <c r="C133" s="2"/>
+      <c r="D133" s="2"/>
     </row>
     <row r="134" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
     </row>
     <row r="135" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C135" s="3"/>
-      <c r="D135" s="3"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
     </row>
     <row r="136" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
     </row>
     <row r="137" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
     </row>
     <row r="138" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C138" s="3"/>
-      <c r="D138" s="3"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
     </row>
     <row r="139" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C139" s="3"/>
-      <c r="D139" s="3"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
     </row>
     <row r="140" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C140" s="3"/>
-      <c r="D140" s="3"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
     </row>
     <row r="141" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
     </row>
     <row r="142" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
     </row>
     <row r="143" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
     </row>
     <row r="144" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
     </row>
     <row r="145" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
     </row>
     <row r="146" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
     </row>
     <row r="147" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C147" s="3"/>
-      <c r="D147" s="3"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
     </row>
     <row r="148" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
     </row>
     <row r="149" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
     </row>
     <row r="150" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C150" s="3"/>
-      <c r="D150" s="3"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
     </row>
     <row r="151" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
     </row>
     <row r="152" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
     </row>
     <row r="153" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
     </row>
     <row r="154" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
     </row>
     <row r="155" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
     </row>
     <row r="156" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
     </row>
     <row r="157" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
     </row>
     <row r="158" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
     </row>
     <row r="159" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
     </row>
     <row r="160" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
     </row>
     <row r="161" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
     </row>
     <row r="162" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
     </row>
     <row r="163" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
     </row>
     <row r="164" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
     </row>
     <row r="165" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
     </row>
     <row r="166" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
     </row>
     <row r="167" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
     </row>
     <row r="168" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
     </row>
     <row r="169" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
     </row>
     <row r="170" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C170" s="3"/>
-      <c r="D170" s="3"/>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
     </row>
     <row r="171" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C171" s="3"/>
-      <c r="D171" s="3"/>
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
     </row>
     <row r="172" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C172" s="3"/>
-      <c r="D172" s="3"/>
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
     </row>
     <row r="173" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C173" s="3"/>
-      <c r="D173" s="3"/>
+      <c r="C173" s="2"/>
+      <c r="D173" s="2"/>
     </row>
     <row r="174" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C174" s="3"/>
-      <c r="D174" s="3"/>
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
     </row>
     <row r="175" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C175" s="3"/>
-      <c r="D175" s="3"/>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
     </row>
     <row r="176" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C176" s="3"/>
-      <c r="D176" s="3"/>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
     </row>
     <row r="177" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C177" s="3"/>
-      <c r="D177" s="3"/>
+      <c r="C177" s="2"/>
+      <c r="D177" s="2"/>
     </row>
     <row r="178" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C178" s="3"/>
-      <c r="D178" s="3"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
     </row>
     <row r="179" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
     </row>
     <row r="180" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
     </row>
     <row r="181" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
     </row>
     <row r="182" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
     </row>
     <row r="183" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C183" s="3"/>
-      <c r="D183" s="3"/>
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
     </row>
     <row r="184" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C184" s="3"/>
-      <c r="D184" s="3"/>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
     </row>
     <row r="185" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
     </row>
     <row r="186" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
     </row>
     <row r="187" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
     </row>
     <row r="188" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
+      <c r="C188" s="2"/>
+      <c r="D188" s="2"/>
     </row>
     <row r="189" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
+      <c r="C189" s="2"/>
+      <c r="D189" s="2"/>
     </row>
     <row r="190" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
+      <c r="C190" s="2"/>
+      <c r="D190" s="2"/>
     </row>
     <row r="191" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C191" s="3"/>
-      <c r="D191" s="3"/>
+      <c r="C191" s="2"/>
+      <c r="D191" s="2"/>
     </row>
     <row r="192" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2"/>
     </row>
     <row r="193" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C193" s="3"/>
-      <c r="D193" s="3"/>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2"/>
     </row>
     <row r="194" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C194" s="3"/>
-      <c r="D194" s="3"/>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
     </row>
     <row r="195" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C195" s="3"/>
-      <c r="D195" s="3"/>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
     </row>
     <row r="196" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2"/>
     </row>
     <row r="197" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
     </row>
     <row r="198" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
     </row>
     <row r="199" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2"/>
     </row>
     <row r="200" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C200" s="3"/>
-      <c r="D200" s="3"/>
+      <c r="C200" s="2"/>
+      <c r="D200" s="2"/>
     </row>
     <row r="201" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C201" s="3"/>
-      <c r="D201" s="3"/>
+      <c r="C201" s="2"/>
+      <c r="D201" s="2"/>
     </row>
     <row r="202" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C202" s="3"/>
-      <c r="D202" s="3"/>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
     </row>
     <row r="203" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C203" s="3"/>
-      <c r="D203" s="3"/>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2"/>
     </row>
     <row r="204" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C204" s="3"/>
-      <c r="D204" s="3"/>
+      <c r="C204" s="2"/>
+      <c r="D204" s="2"/>
     </row>
     <row r="205" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C205" s="3"/>
-      <c r="D205" s="3"/>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
     </row>
     <row r="206" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C206" s="3"/>
-      <c r="D206" s="3"/>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
     </row>
     <row r="207" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C207" s="3"/>
-      <c r="D207" s="3"/>
+      <c r="C207" s="2"/>
+      <c r="D207" s="2"/>
     </row>
     <row r="208" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C208" s="3"/>
-      <c r="D208" s="3"/>
+      <c r="C208" s="2"/>
+      <c r="D208" s="2"/>
     </row>
     <row r="209" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C209" s="3"/>
-      <c r="D209" s="3"/>
+      <c r="C209" s="2"/>
+      <c r="D209" s="2"/>
     </row>
     <row r="210" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C210" s="3"/>
-      <c r="D210" s="3"/>
+      <c r="C210" s="2"/>
+      <c r="D210" s="2"/>
     </row>
     <row r="211" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C211" s="3"/>
-      <c r="D211" s="3"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
     </row>
     <row r="212" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C212" s="3"/>
-      <c r="D212" s="3"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
     </row>
     <row r="213" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C213" s="3"/>
-      <c r="D213" s="3"/>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
     </row>
     <row r="214" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C214" s="3"/>
-      <c r="D214" s="3"/>
+      <c r="C214" s="2"/>
+      <c r="D214" s="2"/>
     </row>
     <row r="215" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C215" s="3"/>
-      <c r="D215" s="3"/>
+      <c r="C215" s="2"/>
+      <c r="D215" s="2"/>
     </row>
     <row r="216" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
     </row>
     <row r="217" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
     </row>
     <row r="218" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
+      <c r="C218" s="2"/>
+      <c r="D218" s="2"/>
     </row>
     <row r="219" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C219" s="3"/>
-      <c r="D219" s="3"/>
+      <c r="C219" s="2"/>
+      <c r="D219" s="2"/>
     </row>
     <row r="220" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
+      <c r="C220" s="2"/>
+      <c r="D220" s="2"/>
     </row>
     <row r="221" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C221" s="3"/>
-      <c r="D221" s="3"/>
+      <c r="C221" s="2"/>
+      <c r="D221" s="2"/>
     </row>
     <row r="222" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C222" s="3"/>
-      <c r="D222" s="3"/>
+      <c r="C222" s="2"/>
+      <c r="D222" s="2"/>
     </row>
     <row r="223" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C223" s="3"/>
-      <c r="D223" s="3"/>
+      <c r="C223" s="2"/>
+      <c r="D223" s="2"/>
     </row>
     <row r="224" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C224" s="3"/>
-      <c r="D224" s="3"/>
+      <c r="C224" s="2"/>
+      <c r="D224" s="2"/>
     </row>
     <row r="225" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C225" s="3"/>
-      <c r="D225" s="3"/>
+      <c r="C225" s="2"/>
+      <c r="D225" s="2"/>
     </row>
     <row r="226" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C226" s="3"/>
-      <c r="D226" s="3"/>
+      <c r="C226" s="2"/>
+      <c r="D226" s="2"/>
     </row>
     <row r="227" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C227" s="3"/>
-      <c r="D227" s="3"/>
+      <c r="C227" s="2"/>
+      <c r="D227" s="2"/>
     </row>
     <row r="228" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C228" s="3"/>
-      <c r="D228" s="3"/>
+      <c r="C228" s="2"/>
+      <c r="D228" s="2"/>
     </row>
     <row r="229" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C229" s="3"/>
-      <c r="D229" s="3"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
     </row>
     <row r="230" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C230" s="3"/>
-      <c r="D230" s="3"/>
+      <c r="C230" s="2"/>
+      <c r="D230" s="2"/>
     </row>
     <row r="231" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C231" s="3"/>
-      <c r="D231" s="3"/>
+      <c r="C231" s="2"/>
+      <c r="D231" s="2"/>
     </row>
     <row r="232" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C232" s="3"/>
-      <c r="D232" s="3"/>
+      <c r="C232" s="2"/>
+      <c r="D232" s="2"/>
     </row>
     <row r="233" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C233" s="3"/>
-      <c r="D233" s="3"/>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
     </row>
     <row r="234" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C234" s="3"/>
-      <c r="D234" s="3"/>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
     </row>
     <row r="235" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C235" s="3"/>
-      <c r="D235" s="3"/>
+      <c r="C235" s="2"/>
+      <c r="D235" s="2"/>
     </row>
     <row r="236" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C236" s="3"/>
-      <c r="D236" s="3"/>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
     </row>
     <row r="237" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C237" s="3"/>
-      <c r="D237" s="3"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
     </row>
     <row r="238" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C238" s="3"/>
-      <c r="D238" s="3"/>
+      <c r="C238" s="2"/>
+      <c r="D238" s="2"/>
     </row>
     <row r="239" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C239" s="3"/>
-      <c r="D239" s="3"/>
+      <c r="C239" s="2"/>
+      <c r="D239" s="2"/>
     </row>
     <row r="240" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C240" s="3"/>
-      <c r="D240" s="3"/>
+      <c r="C240" s="2"/>
+      <c r="D240" s="2"/>
     </row>
     <row r="241" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C241" s="3"/>
-      <c r="D241" s="3"/>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
     </row>
     <row r="242" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C242" s="3"/>
-      <c r="D242" s="3"/>
-    </row>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C242" s="2"/>
+      <c r="D242" s="2"/>
+    </row>
+    <row r="991" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>